<commit_message>
add get idx value and len of idx
</commit_message>
<xml_diff>
--- a/pycode/file/data_w_excel.xlsx
+++ b/pycode/file/data_w_excel.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38753" yWindow="727" windowWidth="15254" windowHeight="9623" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="JDisplacements" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_JD" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_SHEET" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -29,7 +29,9 @@
       <name val="Calibri"/>
       <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -450,16 +452,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B163"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -469,7 +471,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>R3_idx</t>
+          <t>gary</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
         </is>
       </c>
     </row>
@@ -478,27 +495,66 @@
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
+        <is>
+          <t>Hsieh</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>R3</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Radians</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Radians</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Radians</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>w(x)</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -508,6 +564,15 @@
       <c r="B5" t="n">
         <v>0</v>
       </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -516,13 +581,31 @@
       <c r="B6" t="n">
         <v>0</v>
       </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -530,7 +613,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -538,7 +630,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
         <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -548,6 +649,15 @@
       <c r="B10" t="n">
         <v>0</v>
       </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -556,6 +666,15 @@
       <c r="B11" t="n">
         <v>0</v>
       </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -564,6 +683,15 @@
       <c r="B12" t="n">
         <v>0</v>
       </c>
+      <c r="C12" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.472</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -572,6 +700,15 @@
       <c r="B13" t="n">
         <v>0</v>
       </c>
+      <c r="C13" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>20.895</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -580,6 +717,15 @@
       <c r="B14" t="n">
         <v>0</v>
       </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>21.484</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -588,6 +734,15 @@
       <c r="B15" t="n">
         <v>0</v>
       </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>15.206</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -596,6 +751,15 @@
       <c r="B16" t="n">
         <v>0</v>
       </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>15.206</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -604,6 +768,15 @@
       <c r="B17" t="n">
         <v>0</v>
       </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>21.484</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -612,6 +785,15 @@
       <c r="B18" t="n">
         <v>0</v>
       </c>
+      <c r="C18" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20.895</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -620,6 +802,15 @@
       <c r="B19" t="n">
         <v>0</v>
       </c>
+      <c r="C19" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.472</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -628,6 +819,15 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
+      <c r="C20" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.237</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -636,6 +836,15 @@
       <c r="B21" t="n">
         <v>0</v>
       </c>
+      <c r="C21" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>22.073</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -644,6 +853,15 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>22.661</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -652,6 +870,15 @@
       <c r="B23" t="n">
         <v>0</v>
       </c>
+      <c r="C23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17.266</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -660,6 +887,15 @@
       <c r="B24" t="n">
         <v>0</v>
       </c>
+      <c r="C24" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -668,6 +904,15 @@
       <c r="B25" t="n">
         <v>0</v>
       </c>
+      <c r="C25" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -676,6 +921,15 @@
       <c r="B26" t="n">
         <v>0</v>
       </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -684,6 +938,15 @@
       <c r="B27" t="n">
         <v>0</v>
       </c>
+      <c r="C27" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -692,6 +955,15 @@
       <c r="B28" t="n">
         <v>0</v>
       </c>
+      <c r="C28" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -700,6 +972,15 @@
       <c r="B29" t="n">
         <v>0</v>
       </c>
+      <c r="C29" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -708,6 +989,15 @@
       <c r="B30" t="n">
         <v>0</v>
       </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -716,6 +1006,15 @@
       <c r="B31" t="n">
         <v>0</v>
       </c>
+      <c r="C31" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -724,6 +1023,15 @@
       <c r="B32" t="n">
         <v>0</v>
       </c>
+      <c r="C32" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -732,6 +1040,15 @@
       <c r="B33" t="n">
         <v>0</v>
       </c>
+      <c r="C33" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -740,6 +1057,15 @@
       <c r="B34" t="n">
         <v>0</v>
       </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -748,6 +1074,15 @@
       <c r="B35" t="n">
         <v>0</v>
       </c>
+      <c r="C35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -756,6 +1091,15 @@
       <c r="B36" t="n">
         <v>0</v>
       </c>
+      <c r="C36" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.237</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -764,6 +1108,15 @@
       <c r="B37" t="n">
         <v>0</v>
       </c>
+      <c r="C37" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>22.073</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -772,6 +1125,15 @@
       <c r="B38" t="n">
         <v>0</v>
       </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>22.661</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -780,6 +1142,15 @@
       <c r="B39" t="n">
         <v>0</v>
       </c>
+      <c r="C39" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>17.266</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -788,6 +1159,15 @@
       <c r="B40" t="n">
         <v>0</v>
       </c>
+      <c r="C40" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.472</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -796,6 +1176,15 @@
       <c r="B41" t="n">
         <v>0</v>
       </c>
+      <c r="C41" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>20.895</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -804,6 +1193,15 @@
       <c r="B42" t="n">
         <v>0</v>
       </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>21.484</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -812,6 +1210,15 @@
       <c r="B43" t="n">
         <v>0</v>
       </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>15.206</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -820,6 +1227,15 @@
       <c r="B44" t="n">
         <v>0</v>
       </c>
+      <c r="C44" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>17.266</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -828,6 +1244,15 @@
       <c r="B45" t="n">
         <v>0</v>
       </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>22.661</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -836,6 +1261,15 @@
       <c r="B46" t="n">
         <v>0</v>
       </c>
+      <c r="C46" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>22.073</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -844,6 +1278,15 @@
       <c r="B47" t="n">
         <v>0</v>
       </c>
+      <c r="C47" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.237</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -852,6 +1295,15 @@
       <c r="B48" t="n">
         <v>0</v>
       </c>
+      <c r="C48" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -860,6 +1312,15 @@
       <c r="B49" t="n">
         <v>0</v>
       </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -868,6 +1329,15 @@
       <c r="B50" t="n">
         <v>0</v>
       </c>
+      <c r="C50" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -876,6 +1346,15 @@
       <c r="B51" t="n">
         <v>0</v>
       </c>
+      <c r="C51" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -884,6 +1363,15 @@
       <c r="B52" t="n">
         <v>0</v>
       </c>
+      <c r="C52" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -892,6 +1380,15 @@
       <c r="B53" t="n">
         <v>0</v>
       </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -900,6 +1397,15 @@
       <c r="B54" t="n">
         <v>0</v>
       </c>
+      <c r="C54" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -908,6 +1414,15 @@
       <c r="B55" t="n">
         <v>0</v>
       </c>
+      <c r="C55" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -916,6 +1431,15 @@
       <c r="B56" t="n">
         <v>0</v>
       </c>
+      <c r="C56" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>17.168</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -924,6 +1448,15 @@
       <c r="B57" t="n">
         <v>0</v>
       </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>22.465</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -932,6 +1465,15 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
+      <c r="C58" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>21.876</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -940,6 +1482,15 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
+      <c r="C59" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.943</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -948,6 +1499,15 @@
       <c r="B60" t="n">
         <v>0</v>
       </c>
+      <c r="C60" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>17.266</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -956,6 +1516,15 @@
       <c r="B61" t="n">
         <v>0</v>
       </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>22.661</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -964,6 +1533,15 @@
       <c r="B62" t="n">
         <v>0</v>
       </c>
+      <c r="C62" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>22.073</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -972,6 +1550,15 @@
       <c r="B63" t="n">
         <v>0</v>
       </c>
+      <c r="C63" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.237</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -980,6 +1567,15 @@
       <c r="B64" t="n">
         <v>0</v>
       </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>15.206</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -988,6 +1584,15 @@
       <c r="B65" t="n">
         <v>0</v>
       </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>21.484</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -996,6 +1601,15 @@
       <c r="B66" t="n">
         <v>0</v>
       </c>
+      <c r="C66" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>20.895</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1004,6 +1618,15 @@
       <c r="B67" t="n">
         <v>0</v>
       </c>
+      <c r="C67" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.472</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1012,6 +1635,15 @@
       <c r="B68" t="n">
         <v>0</v>
       </c>
+      <c r="C68" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1020,6 +1652,15 @@
       <c r="B69" t="n">
         <v>0</v>
       </c>
+      <c r="C69" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1028,6 +1669,15 @@
       <c r="B70" t="n">
         <v>0</v>
       </c>
+      <c r="C70" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1036,6 +1686,15 @@
       <c r="B71" t="n">
         <v>0</v>
       </c>
+      <c r="C71" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1044,6 +1703,15 @@
       <c r="B72" t="n">
         <v>0</v>
       </c>
+      <c r="C72" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1052,6 +1720,15 @@
       <c r="B73" t="n">
         <v>0</v>
       </c>
+      <c r="C73" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1060,6 +1737,15 @@
       <c r="B74" t="n">
         <v>0</v>
       </c>
+      <c r="C74" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1068,6 +1754,15 @@
       <c r="B75" t="n">
         <v>0</v>
       </c>
+      <c r="C75" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>5.101</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1076,6 +1771,15 @@
       <c r="B76" t="n">
         <v>0</v>
       </c>
+      <c r="C76" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>5.886</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -1084,6 +1788,15 @@
       <c r="B77" t="n">
         <v>0</v>
       </c>
+      <c r="C77" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -1092,6 +1805,15 @@
       <c r="B78" t="n">
         <v>0</v>
       </c>
+      <c r="C78" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -1100,6 +1822,15 @@
       <c r="B79" t="n">
         <v>0</v>
       </c>
+      <c r="C79" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -1108,6 +1839,15 @@
       <c r="B80" t="n">
         <v>0</v>
       </c>
+      <c r="C80" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>5.886</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -1116,6 +1856,15 @@
       <c r="B81" t="n">
         <v>0</v>
       </c>
+      <c r="C81" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" t="n">
+        <v>5.101</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -1124,6 +1873,15 @@
       <c r="B82" t="n">
         <v>0</v>
       </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -1132,6 +1890,15 @@
       <c r="B83" t="n">
         <v>0</v>
       </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -1140,6 +1907,15 @@
       <c r="B84" t="n">
         <v>0</v>
       </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -1148,6 +1924,15 @@
       <c r="B85" t="n">
         <v>0</v>
       </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -1156,6 +1941,15 @@
       <c r="B86" t="n">
         <v>0</v>
       </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -1164,6 +1958,15 @@
       <c r="B87" t="n">
         <v>0</v>
       </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -1172,6 +1975,15 @@
       <c r="B88" t="n">
         <v>0</v>
       </c>
+      <c r="C88" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -1180,6 +1992,15 @@
       <c r="B89" t="n">
         <v>0</v>
       </c>
+      <c r="C89" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -1188,6 +2009,15 @@
       <c r="B90" t="n">
         <v>0</v>
       </c>
+      <c r="C90" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -1196,6 +2026,15 @@
       <c r="B91" t="n">
         <v>0</v>
       </c>
+      <c r="C91" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -1204,6 +2043,15 @@
       <c r="B92" t="n">
         <v>0</v>
       </c>
+      <c r="C92" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -1212,6 +2060,15 @@
       <c r="B93" t="n">
         <v>0</v>
       </c>
+      <c r="C93" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -1220,6 +2077,15 @@
       <c r="B94" t="n">
         <v>0</v>
       </c>
+      <c r="C94" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -1228,6 +2094,15 @@
       <c r="B95" t="n">
         <v>0</v>
       </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -1236,6 +2111,15 @@
       <c r="B96" t="n">
         <v>0</v>
       </c>
+      <c r="C96" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -1244,6 +2128,15 @@
       <c r="B97" t="n">
         <v>0</v>
       </c>
+      <c r="C97" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -1252,6 +2145,15 @@
       <c r="B98" t="n">
         <v>0</v>
       </c>
+      <c r="C98" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -1260,6 +2162,15 @@
       <c r="B99" t="n">
         <v>0</v>
       </c>
+      <c r="C99" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -1268,6 +2179,15 @@
       <c r="B100" t="n">
         <v>0</v>
       </c>
+      <c r="C100" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -1276,6 +2196,15 @@
       <c r="B101" t="n">
         <v>0</v>
       </c>
+      <c r="C101" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -1284,6 +2213,15 @@
       <c r="B102" t="n">
         <v>0</v>
       </c>
+      <c r="C102" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -1292,6 +2230,15 @@
       <c r="B103" t="n">
         <v>0</v>
       </c>
+      <c r="C103" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -1300,6 +2247,15 @@
       <c r="B104" t="n">
         <v>0</v>
       </c>
+      <c r="C104" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -1308,6 +2264,15 @@
       <c r="B105" t="n">
         <v>0</v>
       </c>
+      <c r="C105" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -1316,6 +2281,15 @@
       <c r="B106" t="n">
         <v>0</v>
       </c>
+      <c r="C106" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -1324,6 +2298,15 @@
       <c r="B107" t="n">
         <v>0</v>
       </c>
+      <c r="C107" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -1332,6 +2315,15 @@
       <c r="B108" t="n">
         <v>0</v>
       </c>
+      <c r="C108" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -1340,6 +2332,15 @@
       <c r="B109" t="n">
         <v>0</v>
       </c>
+      <c r="C109" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -1348,6 +2349,15 @@
       <c r="B110" t="n">
         <v>0</v>
       </c>
+      <c r="C110" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -1356,6 +2366,15 @@
       <c r="B111" t="n">
         <v>0</v>
       </c>
+      <c r="C111" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -1364,6 +2383,15 @@
       <c r="B112" t="n">
         <v>0</v>
       </c>
+      <c r="C112" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -1372,6 +2400,15 @@
       <c r="B113" t="n">
         <v>0</v>
       </c>
+      <c r="C113" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -1380,6 +2417,15 @@
       <c r="B114" t="n">
         <v>0</v>
       </c>
+      <c r="C114" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -1388,6 +2434,15 @@
       <c r="B115" t="n">
         <v>0</v>
       </c>
+      <c r="C115" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -1396,6 +2451,15 @@
       <c r="B116" t="n">
         <v>0</v>
       </c>
+      <c r="C116" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>10.399</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -1404,6 +2468,15 @@
       <c r="B117" t="n">
         <v>0</v>
       </c>
+      <c r="C117" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>5.101</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -1412,6 +2485,15 @@
       <c r="B118" t="n">
         <v>0</v>
       </c>
+      <c r="C118" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>5.886</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -1420,6 +2502,15 @@
       <c r="B119" t="n">
         <v>0</v>
       </c>
+      <c r="C119" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -1428,6 +2519,15 @@
       <c r="B120" t="n">
         <v>0</v>
       </c>
+      <c r="C120" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -1436,6 +2536,15 @@
       <c r="B121" t="n">
         <v>0</v>
       </c>
+      <c r="C121" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>5.592</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -1444,6 +2553,15 @@
       <c r="B122" t="n">
         <v>0</v>
       </c>
+      <c r="C122" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>5.886</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -1452,6 +2570,15 @@
       <c r="B123" t="n">
         <v>0</v>
       </c>
+      <c r="C123" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>5.101</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -1460,6 +2587,15 @@
       <c r="B124" t="n">
         <v>0</v>
       </c>
+      <c r="C124" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -1468,6 +2604,15 @@
       <c r="B125" t="n">
         <v>0</v>
       </c>
+      <c r="C125" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -1476,6 +2621,15 @@
       <c r="B126" t="n">
         <v>0</v>
       </c>
+      <c r="C126" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -1484,6 +2638,15 @@
       <c r="B127" t="n">
         <v>0</v>
       </c>
+      <c r="C127" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -1492,6 +2655,15 @@
       <c r="B128" t="n">
         <v>0</v>
       </c>
+      <c r="C128" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D128" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -1500,6 +2672,15 @@
       <c r="B129" t="n">
         <v>0</v>
       </c>
+      <c r="C129" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -1508,6 +2689,15 @@
       <c r="B130" t="n">
         <v>0</v>
       </c>
+      <c r="C130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -1516,6 +2706,15 @@
       <c r="B131" t="n">
         <v>0</v>
       </c>
+      <c r="C131" t="n">
+        <v>0</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -1524,6 +2723,15 @@
       <c r="B132" t="n">
         <v>0</v>
       </c>
+      <c r="C132" t="n">
+        <v>0</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -1532,6 +2740,15 @@
       <c r="B133" t="n">
         <v>0</v>
       </c>
+      <c r="C133" t="n">
+        <v>0</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -1540,6 +2757,15 @@
       <c r="B134" t="n">
         <v>0</v>
       </c>
+      <c r="C134" t="n">
+        <v>0</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -1548,6 +2774,15 @@
       <c r="B135" t="n">
         <v>0</v>
       </c>
+      <c r="C135" t="n">
+        <v>0</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -1556,6 +2791,15 @@
       <c r="B136" t="n">
         <v>0</v>
       </c>
+      <c r="C136" t="n">
+        <v>0</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -1564,6 +2808,15 @@
       <c r="B137" t="n">
         <v>0</v>
       </c>
+      <c r="C137" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -1572,6 +2825,15 @@
       <c r="B138" t="n">
         <v>0</v>
       </c>
+      <c r="C138" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -1580,6 +2842,15 @@
       <c r="B139" t="n">
         <v>0</v>
       </c>
+      <c r="C139" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -1588,6 +2859,15 @@
       <c r="B140" t="n">
         <v>0</v>
       </c>
+      <c r="C140" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -1596,6 +2876,15 @@
       <c r="B141" t="n">
         <v>0</v>
       </c>
+      <c r="C141" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -1604,6 +2893,15 @@
       <c r="B142" t="n">
         <v>0</v>
       </c>
+      <c r="C142" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D142" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -1612,6 +2910,15 @@
       <c r="B143" t="n">
         <v>0</v>
       </c>
+      <c r="C143" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -1620,6 +2927,15 @@
       <c r="B144" t="n">
         <v>0</v>
       </c>
+      <c r="C144" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D144" t="n">
+        <v>0</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -1628,6 +2944,15 @@
       <c r="B145" t="n">
         <v>0</v>
       </c>
+      <c r="C145" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D145" t="n">
+        <v>0</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -1636,6 +2961,15 @@
       <c r="B146" t="n">
         <v>0</v>
       </c>
+      <c r="C146" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D146" t="n">
+        <v>0</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -1644,6 +2978,15 @@
       <c r="B147" t="n">
         <v>0</v>
       </c>
+      <c r="C147" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -1652,6 +2995,15 @@
       <c r="B148" t="n">
         <v>0</v>
       </c>
+      <c r="C148" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -1660,6 +3012,15 @@
       <c r="B149" t="n">
         <v>0</v>
       </c>
+      <c r="C149" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -1668,6 +3029,15 @@
       <c r="B150" t="n">
         <v>0</v>
       </c>
+      <c r="C150" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D150" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -1676,6 +3046,15 @@
       <c r="B151" t="n">
         <v>0</v>
       </c>
+      <c r="C151" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -1684,6 +3063,15 @@
       <c r="B152" t="n">
         <v>0</v>
       </c>
+      <c r="C152" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D152" t="n">
+        <v>0</v>
+      </c>
+      <c r="E152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -1692,6 +3080,15 @@
       <c r="B153" t="n">
         <v>0</v>
       </c>
+      <c r="C153" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D153" t="n">
+        <v>0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -1700,6 +3097,15 @@
       <c r="B154" t="n">
         <v>0</v>
       </c>
+      <c r="C154" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D154" t="n">
+        <v>0</v>
+      </c>
+      <c r="E154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -1708,6 +3114,15 @@
       <c r="B155" t="n">
         <v>0</v>
       </c>
+      <c r="C155" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D155" t="n">
+        <v>0</v>
+      </c>
+      <c r="E155" t="n">
+        <v>31.686</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -1716,6 +3131,15 @@
       <c r="B156" t="n">
         <v>0</v>
       </c>
+      <c r="C156" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -1724,6 +3148,15 @@
       <c r="B157" t="n">
         <v>0</v>
       </c>
+      <c r="C157" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D157" t="n">
+        <v>0</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -1732,6 +3165,15 @@
       <c r="B158" t="n">
         <v>0</v>
       </c>
+      <c r="C158" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -1740,6 +3182,15 @@
       <c r="B159" t="n">
         <v>0</v>
       </c>
+      <c r="C159" t="n">
+        <v>0</v>
+      </c>
+      <c r="D159" t="n">
+        <v>0</v>
+      </c>
+      <c r="E159" t="n">
+        <v>31.686</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -1748,6 +3199,15 @@
       <c r="B160" t="n">
         <v>0</v>
       </c>
+      <c r="C160" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D160" t="n">
+        <v>0</v>
+      </c>
+      <c r="E160" t="n">
+        <v>63.471</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -1756,25 +3216,35 @@
       <c r="B161" t="n">
         <v>0</v>
       </c>
+      <c r="C161" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>63.471</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="1" t="n">
-        <v>161</v>
-      </c>
-      <c r="B163" t="n">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="C162" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D162" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" t="n">
+        <v>63.471</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1784,7 +3254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C164"/>
+  <dimension ref="B2:C163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1800,7 +3270,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>R3_idx</t>
+          <t>gary</t>
         </is>
       </c>
     </row>
@@ -1810,7 +3280,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>Hsieh</t>
         </is>
       </c>
     </row>
@@ -1820,7 +3290,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Radians</t>
+          <t>R1</t>
         </is>
       </c>
     </row>
@@ -1828,8 +3298,10 @@
       <c r="B5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Radians</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1853,7 +3325,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1861,7 +3333,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1869,7 +3341,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3092,20 +4564,8 @@
       <c r="B163" s="2" t="n">
         <v>160</v>
       </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>garyhsieh</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="B164" s="2" t="n">
-        <v>161</v>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>garyhsieh</t>
-        </is>
+      <c r="C163" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>